<commit_message>
Edition with 75k rows
</commit_message>
<xml_diff>
--- a/data/result/error_report.xlsx
+++ b/data/result/error_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,17 +455,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>customer_code</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>invoice_number</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>inv-91</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MISSING_REQUIRED</t>
+          <t>COMPOSITE_DUPLICATE</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -473,27 +477,23 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mandatory field is empty</t>
+          <t>Original row flagged: Conflict with row 447</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>invoice_number</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>customer_code</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>COMPOSITE_DUPLICATE</t>
+          <t>MISSING_REQUIRED</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -501,27 +501,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Original row flagged: Conflict with row 33</t>
+          <t>Mandatory field is empty</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>33</v>
+        <v>402</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>invoice_number</t>
+          <t>customer_code</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>CUST-X</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>COMPOSITE_DUPLICATE</t>
+          <t>PATTERN_MISMATCH</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -529,27 +529,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Duplicate of row 32</t>
+          <t>Invalid pattern: CUST-X</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>199</v>
+        <v>403</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>invoice_number</t>
+          <t>customer_code</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>inv-3197</t>
+          <t>CUST-X</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>COMPOSITE_DUPLICATE</t>
+          <t>PATTERN_MISMATCH</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -557,13 +557,13 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Original row flagged: Conflict with row 205</t>
+          <t>Invalid pattern: CUST-X</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>205</v>
+        <v>447</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>INV-3197</t>
+          <t>INV-91</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -585,95 +585,97 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Duplicate of row 199</t>
+          <t>Duplicate of row 93</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>42</v>
+        <v>503</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>customer_code</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ab</t>
+          <t>CUST-Y</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>BUSINESS_RULE_VIOLATION</t>
+          <t>PATTERN_MISMATCH</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Too short (Min: 3)</t>
+          <t>Invalid pattern: CUST-Y</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>52</v>
+        <v>504</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>customer_code</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>draft</t>
+          <t>CUST-Y</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>BUSINESS_RULE_VIOLATION</t>
+          <t>PATTERN_MISMATCH</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Invalid value. Must be one of: ['active', 'pending', 'closed', 'suspend']</t>
+          <t>Invalid pattern: CUST-Y</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>62</v>
+        <v>505</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
+          <t>customer_code</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CUST-Y</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BUSINESS_RULE_VIOLATION</t>
+          <t>PATTERN_MISMATCH</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Constraint: Since status is suspend, this must be None</t>
+          <t>Invalid pattern: CUST-Y</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>202</v>
+        <v>30</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -682,7 +684,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>German Tech GmbH 199 German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199German Tech GmbH 199</t>
+          <t>CompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompanyCompany 28</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -701,17 +703,21 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>203</v>
+        <v>302</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MISSING_REQUIRED</t>
+          <t>BUSINESS_RULE_VIOLATION</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -719,35 +725,63 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Mandatory field is empty</t>
+          <t>Constraint: Since status is suspend, this must be None</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12</v>
+        <v>703</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>invalid_email.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PATTERN_MISMATCH</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Invalid email format</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>202</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>project_code</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>INVALID-123</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>WRONG-CODE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>PATTERN_MISMATCH</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E13" t="n">
         <v>3</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Invalid pattern: INVALID-123</t>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Invalid pattern: WRONG-CODE</t>
         </is>
       </c>
     </row>

</xml_diff>